<commit_message>
added percentage of locality spending to script
</commit_message>
<xml_diff>
--- a/Input/Locality Spending/levelone21_county.xlsx
+++ b/Input/Locality Spending/levelone21_county.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://esf0-my.sharepoint.com/personal/jmelliot_esf_edu/Documents/Summer 23/754 MPA Workshop/Adirontax Github/Tax Rates &amp; Parcels/Input/Locality Spending/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{9F17455C-3451-41C1-AC49-75BD33FBBB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8797A0F0-B34A-4238-B746-55E665B01C8B}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9F17455C-3451-41C1-AC49-75BD33FBBB6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E225A014-3CB1-4A48-B7F9-35406E3E40AD}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="27580" windowHeight="18460" xr2:uid="{4CE98B25-39F9-49B3-8EEF-2C4C647A6D25}"/>
+    <workbookView xWindow="1460" yWindow="3800" windowWidth="20520" windowHeight="13390" xr2:uid="{4CE98B25-39F9-49B3-8EEF-2C4C647A6D25}"/>
   </bookViews>
   <sheets>
     <sheet name="County" sheetId="4" r:id="rId1"/>
@@ -1161,7 +1161,7 @@
     <col min="41" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:39" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>

</xml_diff>